<commit_message>
Various small other changes
</commit_message>
<xml_diff>
--- a/hardware/tools/diffprobe/simpleversion_eagle/bom_diffprobesimple.xlsx
+++ b/hardware/tools/diffprobe/simpleversion_eagle/bom_diffprobesimple.xlsx
@@ -562,7 +562,7 @@
   <dimension ref="A3:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,7 +915,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -925,7 +925,7 @@
       </c>
       <c r="J19" s="2">
         <f>SUM(J4:J18)</f>
-        <v>13.688000000000001</v>
+        <v>15.688000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>